<commit_message>
forgot to add detail
</commit_message>
<xml_diff>
--- a/roadtrip.xlsx
+++ b/roadtrip.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marzaric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marzaric\GBP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Day 1</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Cayo Costa-- WATCH THE ECLIPSE</t>
+  </si>
+  <si>
+    <t>drive to for myers and restock</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +658,9 @@
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
addede the new packing list and modifications to ecel and forsale
</commit_message>
<xml_diff>
--- a/roadtrip.xlsx
+++ b/roadtrip.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13890"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Option 1-Grand Canyon" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Day 1</t>
   </si>
@@ -150,15 +150,9 @@
     <t>john pennekamp SP</t>
   </si>
   <si>
-    <t>drive to key west. Bahia honda state park</t>
-  </si>
-  <si>
     <t>leave fort myers/tampa arrive and spend day in nashville</t>
   </si>
   <si>
-    <t>leave bahia honda state Park. Go to boyds (???)</t>
-  </si>
-  <si>
     <t>depart to Cayo Costa State park (ferry leavess at 2)</t>
   </si>
   <si>
@@ -169,6 +163,12 @@
   </si>
   <si>
     <t>drive to for myers and restock</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>pennekamp</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,9 +622,11 @@
       <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -632,14 +634,16 @@
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -647,9 +651,11 @@
         <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -659,7 +665,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -671,7 +677,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -683,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -695,7 +701,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -707,7 +713,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
     </row>

</xml_diff>